<commit_message>
Updated STD and ABSA code finding procedures.
</commit_message>
<xml_diff>
--- a/temp/final_output_CAPITEC.xlsx
+++ b/temp/final_output_CAPITEC.xlsx
@@ -592,7 +592,11 @@
           <t xml:space="preserve">EFT WAGES SEEL D583C 31DEC24                                </t>
         </is>
       </c>
-      <c r="C7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>D583</t>
+        </is>
+      </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="n">
         <v>35583.67</v>
@@ -3802,10 +3806,8 @@
       </c>
       <c r="C123" t="inlineStr"/>
       <c r="D123" t="inlineStr"/>
-      <c r="E123" t="inlineStr">
-        <is>
-          <t>-730</t>
-        </is>
+      <c r="E123" t="n">
+        <v>-730</v>
       </c>
       <c r="F123" t="n">
         <v>0</v>

</xml_diff>